<commit_message>
Mark done in front of completed question in the list
</commit_message>
<xml_diff>
--- a/DSA-Questions.xlsx
+++ b/DSA-Questions.xlsx
@@ -1429,7 +1429,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1491,13 +1491,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1513,7 +1526,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1537,6 +1550,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1544,6 +1560,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1844,7 +1865,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1854,8 +1875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1916,7 +1937,7 @@
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="7">

</xml_diff>

<commit_message>
After completing problem 1 of Array, question bank updated.
</commit_message>
<xml_diff>
--- a/DSA-Questions.xlsx
+++ b/DSA-Questions.xlsx
@@ -1865,7 +1865,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1876,7 +1876,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1923,7 +1923,7 @@
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="7">

</xml_diff>

<commit_message>
Log file updated after solving problem 4
</commit_message>
<xml_diff>
--- a/DSA-Questions.xlsx
+++ b/DSA-Questions.xlsx
@@ -1432,7 +1432,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1502,6 +1502,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1530,7 +1537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1555,6 +1562,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1869,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1880,7 +1890,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1969,8 +1979,8 @@
       <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>4</v>
+      <c r="C9" s="12" t="s">
+        <v>466</v>
       </c>
       <c r="D9" s="7">
         <v>4</v>

</xml_diff>

<commit_message>
Question bank updated after solving problem 3.
</commit_message>
<xml_diff>
--- a/DSA-Questions.xlsx
+++ b/DSA-Questions.xlsx
@@ -1879,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1890,7 +1890,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1965,8 +1965,8 @@
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>4</v>
+      <c r="C8" s="12" t="s">
+        <v>466</v>
       </c>
       <c r="D8" s="7">
         <v>3</v>

</xml_diff>

<commit_message>
Question bank updated after solving problem 5
</commit_message>
<xml_diff>
--- a/DSA-Questions.xlsx
+++ b/DSA-Questions.xlsx
@@ -1879,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1993,8 +1993,8 @@
       <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>4</v>
+      <c r="C10" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D10" s="7">
         <v>5</v>

</xml_diff>

<commit_message>
Question bank updated after solving problem 7
</commit_message>
<xml_diff>
--- a/DSA-Questions.xlsx
+++ b/DSA-Questions.xlsx
@@ -1879,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1890,7 +1890,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2021,8 +2021,8 @@
       <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
+      <c r="C12" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D12" s="7">
         <v>7</v>

</xml_diff>